<commit_message>
fix defaulted customers template
</commit_message>
<xml_diff>
--- a/src/Mohassel/Assets/sheets/defaulted-customers-template.xlsx
+++ b/src/Mohassel/Assets/sheets/defaulted-customers-template.xlsx
@@ -13,7 +13,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -180,11 +180,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="166" formatCode="@"/>
-    <numFmt numFmtId="167" formatCode="D/M/YYYY"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -310,7 +308,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -319,27 +317,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -420,17 +406,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V1048576"/>
+  <dimension ref="A1:V65534"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="ALX1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AMH8" activeCellId="0" sqref="AMH8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="25.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="25.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="9" style="0" width="25.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="1" style="1" width="25.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="14.44"/>
   </cols>
   <sheetData>
@@ -456,7 +440,7 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
@@ -465,7 +449,7 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="4" t="s">
@@ -477,7 +461,7 @@
       <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="P1" s="4" t="s">
@@ -486,7 +470,7 @@
       <c r="Q1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="S1" s="4" t="s">
@@ -502,7 +486,6 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -718,8 +701,8 @@
     <row r="215" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="216" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="217" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="219" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1498,9 +1481,7 @@
     <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65534" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
- Replace defaulting customers excel file - Add two field to customer action form: finalVerdict and finalVerdictDate
</commit_message>
<xml_diff>
--- a/src/Mohassel/Assets/sheets/defaulted-customers-template.xlsx
+++ b/src/Mohassel/Assets/sheets/defaulted-customers-template.xlsx
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t xml:space="preserve">الرقم القومي</t>
   </si>
@@ -175,16 +175,41 @@
   <si>
     <t xml:space="preserve">حاله الدعوي ملخص</t>
   </si>
+  <si>
+    <t xml:space="preserve">الحكم النهائي </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="14"/>
+        <color rgb="FFEEEEEE"/>
+        <rFont val="Book Antiqua"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">تاريخ الحكم النهائي </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFEEEEEE"/>
+        <rFont val="Book Antiqua"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(dd/mm/yyyy) </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="166" formatCode="@"/>
-    <numFmt numFmtId="167" formatCode="D/M/YYYY"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -310,7 +335,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -319,27 +344,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -420,18 +433,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V1048576"/>
+  <dimension ref="A1:X65534"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="ALX1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AMH8" activeCellId="0" sqref="AMH8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W13" activeCellId="0" sqref="W13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="25.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="25.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="9" style="0" width="25.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="1" style="1" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="22.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="14.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -456,7 +469,7 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
@@ -465,7 +478,7 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="4" t="s">
@@ -477,7 +490,7 @@
       <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="P1" s="4" t="s">
@@ -486,7 +499,7 @@
       <c r="Q1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="S1" s="4" t="s">
@@ -501,8 +514,13 @@
       <c r="V1" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="W1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -718,8 +736,8 @@
     <row r="215" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="216" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="217" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="219" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1498,9 +1516,7 @@
     <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65534" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Add fields for defaulted customers template excel sheet
</commit_message>
<xml_diff>
--- a/src/Mohassel/Assets/sheets/defaulted-customers-template.xlsx
+++ b/src/Mohassel/Assets/sheets/defaulted-customers-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t xml:space="preserve">الرقم القومي</t>
   </si>
@@ -174,6 +174,36 @@
   </si>
   <si>
     <t xml:space="preserve">حاله الدعوي ملخص</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الحكم النهائي </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="14"/>
+        <color rgb="FFEEEEEE"/>
+        <rFont val="Book Antiqua"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">تاريخ الحكم النهائي </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFEEEEEE"/>
+        <rFont val="Book Antiqua"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(dd/mm/yyyy) </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">رقم الحصر النهائي</t>
   </si>
 </sst>
 </file>
@@ -406,16 +436,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V65534"/>
+  <dimension ref="A1:Y65534"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="1" style="1" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="22.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="14.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -484,6 +517,15 @@
       </c>
       <c r="V1" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Revert "Merge remote-tracking branch 'upstream/einshams-v2' into enhancements/halan-integration"
This reverts commit a678a75f4aadf3f08c9cba6aa4f25cf215f70ac7, reversing
changes made to 0666ba9395dc0456f8af55e34ec47a81811aee20.
</commit_message>
<xml_diff>
--- a/src/Mohassel/Assets/sheets/defaulted-customers-template.xlsx
+++ b/src/Mohassel/Assets/sheets/defaulted-customers-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t xml:space="preserve">الرقم القومي</t>
   </si>
@@ -201,9 +201,6 @@
       </rPr>
       <t xml:space="preserve">(dd/mm/yyyy) </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">رقم الحصر النهائي</t>
   </si>
 </sst>
 </file>
@@ -436,19 +433,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y65534"/>
+  <dimension ref="A1:X65534"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W13" activeCellId="0" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="1" style="1" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="22.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="14.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="22.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="14.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -523,9 +519,6 @@
       </c>
       <c r="X1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge remote-tracking branch 'upstream/einshams-v2' into enhancements/halan-integration""
This reverts commit 23d4003e7a7e0af089f7988f6cefe11162b54434.
</commit_message>
<xml_diff>
--- a/src/Mohassel/Assets/sheets/defaulted-customers-template.xlsx
+++ b/src/Mohassel/Assets/sheets/defaulted-customers-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t xml:space="preserve">الرقم القومي</t>
   </si>
@@ -201,6 +201,9 @@
       </rPr>
       <t xml:space="preserve">(dd/mm/yyyy) </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">رقم الحصر النهائي</t>
   </si>
 </sst>
 </file>
@@ -433,18 +436,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X65534"/>
+  <dimension ref="A1:Y65534"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W13" activeCellId="0" sqref="W13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="1" style="1" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="14.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="22.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="22.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="14.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -519,6 +523,9 @@
       </c>
       <c r="X1" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>